<commit_message>
formalização planilhas com muitos dados
</commit_message>
<xml_diff>
--- a/planilhas/falhas.xlsx
+++ b/planilhas/falhas.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
   <si>
     <t>ID*</t>
   </si>
@@ -36,6 +36,9 @@
   </si>
   <si>
     <t>Problema(s)</t>
+  </si>
+  <si>
+    <t>id invalido</t>
   </si>
 </sst>
 </file>
@@ -374,7 +377,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -403,6 +406,176 @@
       </c>
       <c r="G1" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2"/>
+      <c r="B2"/>
+      <c r="C2"/>
+      <c r="D2"/>
+      <c r="E2"/>
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3"/>
+      <c r="B3"/>
+      <c r="C3"/>
+      <c r="D3"/>
+      <c r="E3"/>
+      <c r="F3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4"/>
+      <c r="B4"/>
+      <c r="C4"/>
+      <c r="D4"/>
+      <c r="E4"/>
+      <c r="F4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5"/>
+      <c r="B5"/>
+      <c r="C5"/>
+      <c r="D5"/>
+      <c r="E5"/>
+      <c r="F5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6"/>
+      <c r="B6"/>
+      <c r="C6"/>
+      <c r="D6"/>
+      <c r="E6"/>
+      <c r="F6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7"/>
+      <c r="B7"/>
+      <c r="C7"/>
+      <c r="D7"/>
+      <c r="E7"/>
+      <c r="F7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8"/>
+      <c r="B8"/>
+      <c r="C8"/>
+      <c r="D8"/>
+      <c r="E8"/>
+      <c r="F8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9"/>
+      <c r="B9"/>
+      <c r="C9"/>
+      <c r="D9"/>
+      <c r="E9"/>
+      <c r="F9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10"/>
+      <c r="B10"/>
+      <c r="C10"/>
+      <c r="D10"/>
+      <c r="E10"/>
+      <c r="F10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11"/>
+      <c r="B11"/>
+      <c r="C11"/>
+      <c r="D11"/>
+      <c r="E11"/>
+      <c r="F11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12"/>
+      <c r="B12"/>
+      <c r="C12"/>
+      <c r="D12"/>
+      <c r="E12"/>
+      <c r="F12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13"/>
+      <c r="B13"/>
+      <c r="C13"/>
+      <c r="D13"/>
+      <c r="E13"/>
+      <c r="F13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14"/>
+      <c r="B14"/>
+      <c r="C14"/>
+      <c r="D14"/>
+      <c r="E14"/>
+      <c r="F14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15"/>
+      <c r="B15"/>
+      <c r="C15"/>
+      <c r="D15"/>
+      <c r="E15"/>
+      <c r="F15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16"/>
+      <c r="B16"/>
+      <c r="C16"/>
+      <c r="D16"/>
+      <c r="E16"/>
+      <c r="F16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17"/>
+      <c r="B17"/>
+      <c r="C17"/>
+      <c r="D17"/>
+      <c r="E17"/>
+      <c r="F17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18"/>
+      <c r="B18"/>
+      <c r="C18"/>
+      <c r="D18"/>
+      <c r="E18"/>
+      <c r="F18" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bug tarefa e depósito kkk
</commit_message>
<xml_diff>
--- a/planilhas/falhas.xlsx
+++ b/planilhas/falhas.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="7">
   <si>
     <t>ID*</t>
   </si>
@@ -36,9 +36,6 @@
   </si>
   <si>
     <t>Problema(s)</t>
-  </si>
-  <si>
-    <t>id invalido</t>
   </si>
 </sst>
 </file>
@@ -377,7 +374,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -406,226 +403,6 @@
       </c>
       <c r="G1" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2"/>
-      <c r="B2"/>
-      <c r="C2"/>
-      <c r="D2"/>
-      <c r="E2"/>
-      <c r="F2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3"/>
-      <c r="B3"/>
-      <c r="C3"/>
-      <c r="D3"/>
-      <c r="E3"/>
-      <c r="F3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4"/>
-      <c r="B4"/>
-      <c r="C4"/>
-      <c r="D4"/>
-      <c r="E4"/>
-      <c r="F4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5"/>
-      <c r="B5"/>
-      <c r="C5"/>
-      <c r="D5"/>
-      <c r="E5"/>
-      <c r="F5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6"/>
-      <c r="B6"/>
-      <c r="C6"/>
-      <c r="D6"/>
-      <c r="E6"/>
-      <c r="F6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7"/>
-      <c r="B7"/>
-      <c r="C7"/>
-      <c r="D7"/>
-      <c r="E7"/>
-      <c r="F7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8"/>
-      <c r="B8"/>
-      <c r="C8"/>
-      <c r="D8"/>
-      <c r="E8"/>
-      <c r="F8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9"/>
-      <c r="B9"/>
-      <c r="C9"/>
-      <c r="D9"/>
-      <c r="E9"/>
-      <c r="F9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10"/>
-      <c r="B10"/>
-      <c r="C10"/>
-      <c r="D10"/>
-      <c r="E10"/>
-      <c r="F10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11"/>
-      <c r="B11"/>
-      <c r="C11"/>
-      <c r="D11"/>
-      <c r="E11"/>
-      <c r="F11" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12"/>
-      <c r="B12"/>
-      <c r="C12"/>
-      <c r="D12"/>
-      <c r="E12"/>
-      <c r="F12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13"/>
-      <c r="B13"/>
-      <c r="C13"/>
-      <c r="D13"/>
-      <c r="E13"/>
-      <c r="F13" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14"/>
-      <c r="B14"/>
-      <c r="C14"/>
-      <c r="D14"/>
-      <c r="E14"/>
-      <c r="F14" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15"/>
-      <c r="B15"/>
-      <c r="C15"/>
-      <c r="D15"/>
-      <c r="E15"/>
-      <c r="F15" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16"/>
-      <c r="B16"/>
-      <c r="C16"/>
-      <c r="D16"/>
-      <c r="E16"/>
-      <c r="F16" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17"/>
-      <c r="B17"/>
-      <c r="C17"/>
-      <c r="D17"/>
-      <c r="E17"/>
-      <c r="F17" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18"/>
-      <c r="B18"/>
-      <c r="C18"/>
-      <c r="D18"/>
-      <c r="E18"/>
-      <c r="F18" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19"/>
-      <c r="B19"/>
-      <c r="C19"/>
-      <c r="D19"/>
-      <c r="E19"/>
-      <c r="F19" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20"/>
-      <c r="B20"/>
-      <c r="C20"/>
-      <c r="D20"/>
-      <c r="E20"/>
-      <c r="F20" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21"/>
-      <c r="B21"/>
-      <c r="C21"/>
-      <c r="D21"/>
-      <c r="E21"/>
-      <c r="F21" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22"/>
-      <c r="B22"/>
-      <c r="C22"/>
-      <c r="D22"/>
-      <c r="E22"/>
-      <c r="F22" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23"/>
-      <c r="B23"/>
-      <c r="C23"/>
-      <c r="D23"/>
-      <c r="E23"/>
-      <c r="F23" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix alteraçao tab tarefa
</commit_message>
<xml_diff>
--- a/planilhas/falhas.xlsx
+++ b/planilhas/falhas.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="7">
   <si>
     <t>ID*</t>
   </si>
@@ -36,9 +36,6 @@
   </si>
   <si>
     <t>Problema(s)</t>
-  </si>
-  <si>
-    <t>id invalido</t>
   </si>
 </sst>
 </file>
@@ -377,7 +374,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -406,226 +403,6 @@
       </c>
       <c r="G1" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2"/>
-      <c r="B2"/>
-      <c r="C2"/>
-      <c r="D2"/>
-      <c r="E2"/>
-      <c r="F2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3"/>
-      <c r="B3"/>
-      <c r="C3"/>
-      <c r="D3"/>
-      <c r="E3"/>
-      <c r="F3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4"/>
-      <c r="B4"/>
-      <c r="C4"/>
-      <c r="D4"/>
-      <c r="E4"/>
-      <c r="F4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5"/>
-      <c r="B5"/>
-      <c r="C5"/>
-      <c r="D5"/>
-      <c r="E5"/>
-      <c r="F5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6"/>
-      <c r="B6"/>
-      <c r="C6"/>
-      <c r="D6"/>
-      <c r="E6"/>
-      <c r="F6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7"/>
-      <c r="B7"/>
-      <c r="C7"/>
-      <c r="D7"/>
-      <c r="E7"/>
-      <c r="F7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8"/>
-      <c r="B8"/>
-      <c r="C8"/>
-      <c r="D8"/>
-      <c r="E8"/>
-      <c r="F8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9"/>
-      <c r="B9"/>
-      <c r="C9"/>
-      <c r="D9"/>
-      <c r="E9"/>
-      <c r="F9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10"/>
-      <c r="B10"/>
-      <c r="C10"/>
-      <c r="D10"/>
-      <c r="E10"/>
-      <c r="F10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11"/>
-      <c r="B11"/>
-      <c r="C11"/>
-      <c r="D11"/>
-      <c r="E11"/>
-      <c r="F11" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12"/>
-      <c r="B12"/>
-      <c r="C12"/>
-      <c r="D12"/>
-      <c r="E12"/>
-      <c r="F12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13"/>
-      <c r="B13"/>
-      <c r="C13"/>
-      <c r="D13"/>
-      <c r="E13"/>
-      <c r="F13" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14"/>
-      <c r="B14"/>
-      <c r="C14"/>
-      <c r="D14"/>
-      <c r="E14"/>
-      <c r="F14" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15"/>
-      <c r="B15"/>
-      <c r="C15"/>
-      <c r="D15"/>
-      <c r="E15"/>
-      <c r="F15" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16"/>
-      <c r="B16"/>
-      <c r="C16"/>
-      <c r="D16"/>
-      <c r="E16"/>
-      <c r="F16" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17"/>
-      <c r="B17"/>
-      <c r="C17"/>
-      <c r="D17"/>
-      <c r="E17"/>
-      <c r="F17" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18"/>
-      <c r="B18"/>
-      <c r="C18"/>
-      <c r="D18"/>
-      <c r="E18"/>
-      <c r="F18" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19"/>
-      <c r="B19"/>
-      <c r="C19"/>
-      <c r="D19"/>
-      <c r="E19"/>
-      <c r="F19" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20"/>
-      <c r="B20"/>
-      <c r="C20"/>
-      <c r="D20"/>
-      <c r="E20"/>
-      <c r="F20" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21"/>
-      <c r="B21"/>
-      <c r="C21"/>
-      <c r="D21"/>
-      <c r="E21"/>
-      <c r="F21" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22"/>
-      <c r="B22"/>
-      <c r="C22"/>
-      <c r="D22"/>
-      <c r="E22"/>
-      <c r="F22" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23"/>
-      <c r="B23"/>
-      <c r="C23"/>
-      <c r="D23"/>
-      <c r="E23"/>
-      <c r="F23" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix upload planilhas grandes
</commit_message>
<xml_diff>
--- a/planilhas/falhas.xlsx
+++ b/planilhas/falhas.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="7">
   <si>
     <t>ID*</t>
   </si>
@@ -36,9 +36,6 @@
   </si>
   <si>
     <t>Problema(s)</t>
-  </si>
-  <si>
-    <t>id invalido</t>
   </si>
 </sst>
 </file>
@@ -377,7 +374,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -406,176 +403,6 @@
       </c>
       <c r="G1" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2"/>
-      <c r="B2"/>
-      <c r="C2"/>
-      <c r="D2"/>
-      <c r="E2"/>
-      <c r="F2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3"/>
-      <c r="B3"/>
-      <c r="C3"/>
-      <c r="D3"/>
-      <c r="E3"/>
-      <c r="F3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4"/>
-      <c r="B4"/>
-      <c r="C4"/>
-      <c r="D4"/>
-      <c r="E4"/>
-      <c r="F4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5"/>
-      <c r="B5"/>
-      <c r="C5"/>
-      <c r="D5"/>
-      <c r="E5"/>
-      <c r="F5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6"/>
-      <c r="B6"/>
-      <c r="C6"/>
-      <c r="D6"/>
-      <c r="E6"/>
-      <c r="F6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7"/>
-      <c r="B7"/>
-      <c r="C7"/>
-      <c r="D7"/>
-      <c r="E7"/>
-      <c r="F7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8"/>
-      <c r="B8"/>
-      <c r="C8"/>
-      <c r="D8"/>
-      <c r="E8"/>
-      <c r="F8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9"/>
-      <c r="B9"/>
-      <c r="C9"/>
-      <c r="D9"/>
-      <c r="E9"/>
-      <c r="F9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10"/>
-      <c r="B10"/>
-      <c r="C10"/>
-      <c r="D10"/>
-      <c r="E10"/>
-      <c r="F10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11"/>
-      <c r="B11"/>
-      <c r="C11"/>
-      <c r="D11"/>
-      <c r="E11"/>
-      <c r="F11" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12"/>
-      <c r="B12"/>
-      <c r="C12"/>
-      <c r="D12"/>
-      <c r="E12"/>
-      <c r="F12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13"/>
-      <c r="B13"/>
-      <c r="C13"/>
-      <c r="D13"/>
-      <c r="E13"/>
-      <c r="F13" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14"/>
-      <c r="B14"/>
-      <c r="C14"/>
-      <c r="D14"/>
-      <c r="E14"/>
-      <c r="F14" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15"/>
-      <c r="B15"/>
-      <c r="C15"/>
-      <c r="D15"/>
-      <c r="E15"/>
-      <c r="F15" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16"/>
-      <c r="B16"/>
-      <c r="C16"/>
-      <c r="D16"/>
-      <c r="E16"/>
-      <c r="F16" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17"/>
-      <c r="B17"/>
-      <c r="C17"/>
-      <c r="D17"/>
-      <c r="E17"/>
-      <c r="F17" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18"/>
-      <c r="B18"/>
-      <c r="C18"/>
-      <c r="D18"/>
-      <c r="E18"/>
-      <c r="F18" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>